<commit_message>
Attendance for a new day has been added
</commit_message>
<xml_diff>
--- a/PHP Server/Microprocessor_Section_A.xlsx
+++ b/PHP Server/Microprocessor_Section_A.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>2019/11/28</t>
+  </si>
+  <si>
+    <t>2019/11/30</t>
   </si>
   <si>
     <t>17-00001-1</t>
@@ -449,7 +452,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="M16" sqref="M16"/>
@@ -466,7 +469,7 @@
     <col min="7" max="7" width="13.33203125" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,19 +494,22 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -517,19 +523,22 @@
       <c r="H2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>3.9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -543,19 +552,22 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>3.9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -569,19 +581,22 @@
       <c r="H4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>3.9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -595,19 +610,22 @@
       <c r="H5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>3.9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -621,19 +639,22 @@
       <c r="H6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>3.9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -647,19 +668,22 @@
       <c r="H7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>3.9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -673,19 +697,22 @@
       <c r="H8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -697,6 +724,9 @@
         <v>1</v>
       </c>
       <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
     </row>

</xml_diff>